<commit_message>
Funktionierende Version - PWM wird erzeugt, ändern per Socket geht
</commit_message>
<xml_diff>
--- a/growbox-controller/STM32f4_GCU/Documentation/SignalMapping.xlsx
+++ b/growbox-controller/STM32f4_GCU/Documentation/SignalMapping.xlsx
@@ -8,24 +8,36 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\GrowBox_NG\growbox-controller\STM32f4_GCU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F70DA92-67B4-459E-9F08-BC24A4692DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0426564D-E5DF-4E30-BCBD-77C1E3FFC101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="194" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Stecker" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>SPI1_MOSI</t>
   </si>
@@ -33,18 +45,9 @@
     <t>SPI1_SCK</t>
   </si>
   <si>
-    <t>A5</t>
-  </si>
-  <si>
-    <t>A7</t>
-  </si>
-  <si>
     <t>SPI1_MISO</t>
   </si>
   <si>
-    <t>A6</t>
-  </si>
-  <si>
     <t>W5500 ChipSelect</t>
   </si>
   <si>
@@ -94,13 +97,187 @@
   </si>
   <si>
     <t>PA2</t>
+  </si>
+  <si>
+    <t># W5500</t>
+  </si>
+  <si>
+    <t># LEDs</t>
+  </si>
+  <si>
+    <t># UART</t>
+  </si>
+  <si>
+    <t># PUMPS</t>
+  </si>
+  <si>
+    <t>IN1</t>
+  </si>
+  <si>
+    <t>IN2</t>
+  </si>
+  <si>
+    <t>IN3</t>
+  </si>
+  <si>
+    <t>IN4</t>
+  </si>
+  <si>
+    <t>Enable A (PWM)</t>
+  </si>
+  <si>
+    <t>Enable B (PWM)</t>
+  </si>
+  <si>
+    <t>PB13</t>
+  </si>
+  <si>
+    <t>PB15</t>
+  </si>
+  <si>
+    <t>PC2</t>
+  </si>
+  <si>
+    <t>B6</t>
+  </si>
+  <si>
+    <t>B7</t>
+  </si>
+  <si>
+    <t>P1_37</t>
+  </si>
+  <si>
+    <t>P1_39</t>
+  </si>
+  <si>
+    <t>P1_10</t>
+  </si>
+  <si>
+    <t>P1_20</t>
+  </si>
+  <si>
+    <t>P1_19</t>
+  </si>
+  <si>
+    <t>GPIO</t>
+  </si>
+  <si>
+    <t>P1_13</t>
+  </si>
+  <si>
+    <t>P1_14</t>
+  </si>
+  <si>
+    <t>P2_23</t>
+  </si>
+  <si>
+    <t>P2_24</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>P2_25</t>
+  </si>
+  <si>
+    <t>P2_26</t>
+  </si>
+  <si>
+    <t>P2_27</t>
+  </si>
+  <si>
+    <t>P2_28</t>
+  </si>
+  <si>
+    <t># LIGHTS</t>
+  </si>
+  <si>
+    <t>LIGHT_DIM</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>P2_45</t>
+  </si>
+  <si>
+    <t>STROM Einn</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>Gelb</t>
+  </si>
+  <si>
+    <t>GND</t>
+  </si>
+  <si>
+    <t># SENSORS</t>
+  </si>
+  <si>
+    <t>SENSOR_OBEN</t>
+  </si>
+  <si>
+    <t>SENSOR_UNTEN</t>
+  </si>
+  <si>
+    <t>P2_43</t>
+  </si>
+  <si>
+    <t>P2_44</t>
+  </si>
+  <si>
+    <t>A8</t>
+  </si>
+  <si>
+    <t>A9</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>PUMP1_ENABLE</t>
+  </si>
+  <si>
+    <t>PUMP2_ENABLE</t>
+  </si>
+  <si>
+    <t>PUMP1_IN1</t>
+  </si>
+  <si>
+    <t>PUMP1_IN2</t>
+  </si>
+  <si>
+    <t>PUMP2_IN1</t>
+  </si>
+  <si>
+    <t>PUMP2_IN2</t>
+  </si>
+  <si>
+    <t>LED_DIM</t>
+  </si>
+  <si>
+    <t>WATER_OBEN</t>
+  </si>
+  <si>
+    <t>WATER_UNTEN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,6 +290,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF3A3A3A"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -135,8 +318,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -152,6 +344,212 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>208084</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>161087</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>94936</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>94412</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D473B8DD-7931-EED8-E50F-071870341D27}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12571534" y="542087"/>
+          <a:ext cx="11469252" cy="8753475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1026" name="AutoShape 2" descr="L298N Motor Driver Module Pinout">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18DA5EE8-C5A4-9106-322A-4986C4351194}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8705850" y="10344150"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1027" name="AutoShape 3" descr="L298N Motor Driver Module Pinout">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A76FE28F-047F-053C-5A8A-F2D9E1374E0C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="13582650" y="9963150"/>
+          <a:ext cx="6296025" cy="4362450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1667988</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>35627</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>231374</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>79901</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Grafik 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99D96FAB-9970-878A-CA0D-A4AE3352420E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6630513" y="797627"/>
+          <a:ext cx="6535811" cy="5054424"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -417,114 +815,345 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:B13"/>
+  <dimension ref="A2:L54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="C17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B18" t="s">
         <v>19</v>
       </c>
-      <c r="B12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" t="s">
-        <v>22</v>
+      <c r="C18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" t="s">
+        <v>56</v>
+      </c>
+      <c r="D30" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" t="s">
+        <v>64</v>
+      </c>
+      <c r="D34" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" t="s">
+        <v>65</v>
+      </c>
+      <c r="D35" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="54" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L54" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB136EC6-015F-44FE-91D0-47070FF5190A}">
+  <dimension ref="A3:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" t="str">
+        <f>+"12V"</f>
+        <v>12V</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
funktionen zum msg parsen ausgelagert in task_network.c - UNGETESTET
</commit_message>
<xml_diff>
--- a/growbox-controller/STM32f4_GCU/Documentation/SignalMapping.xlsx
+++ b/growbox-controller/STM32f4_GCU/Documentation/SignalMapping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\GrowBox_NG\growbox-controller\STM32f4_GCU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0426564D-E5DF-4E30-BCBD-77C1E3FFC101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3AD9D12-5F9B-4FA2-9A42-1DE76FF20AF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="194" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -818,7 +818,7 @@
   <dimension ref="A2:L54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>